<commit_message>
tests: update platform tests and several expected results files
</commit_message>
<xml_diff>
--- a/tests/expected_results/result_test_download_grupeer_statement_no_cfs.xlsx
+++ b/tests/expected_results/result_test_download_grupeer_statement_no_cfs.xlsx
@@ -1,96 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Account statement" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Account statement" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Transaction ID</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>GRP</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="0"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="5">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf xfId="0" fontId="0" numFmtId="2" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -169,6 +165,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -203,6 +200,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -378,70 +376,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" xSplit="0" ySplit="1"/>
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="D1" activeCellId="0" pane="bottomLeft" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="2" min="1" style="2" width="5.86"/>
-    <col customWidth="1" max="3" min="3" style="3" width="13.99"/>
-    <col customWidth="1" max="4" min="4" style="3" width="8.140000000000001"/>
-    <col customWidth="1" max="5" min="5" style="2" width="9.289999999999999"/>
-    <col customWidth="1" max="6" min="6" style="2" width="10.57"/>
-    <col customWidth="1" max="7" min="7" style="2" width="4.57"/>
-    <col customWidth="1" max="1025" min="8" style="2" width="8.67"/>
+    <col min="3" max="3" width="5.855713" bestFit="true" customWidth="true" style="1"/>
+    <col min="4" max="4" width="13.996582" bestFit="true" customWidth="true" style="1"/>
+    <col min="1" max="1" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="4.570313" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="14.4" r="1" s="4">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>Amount</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Balance</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Currency</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>GRP</t>
-        </is>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="0" footer="0.511805555555555" header="0.511805555555555" left="0" right="0" top="0"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>